<commit_message>
Moving IST training report to extensions DLL
</commit_message>
<xml_diff>
--- a/ESAR.Extensions/templates/trainingReport.xlsx
+++ b/ESAR.Extensions/templates/trainingReport.xlsx
@@ -82,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -126,8 +126,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,13 +432,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,11 +513,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="N2" s="5">
-        <v>42403</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>